<commit_message>
Program 11 - 17
</commit_message>
<xml_diff>
--- a/Questions/Questions.xlsx
+++ b/Questions/Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\GitHub\Programming\Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FA7B7F-576C-4404-AB70-041539B39174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75E173D-5823-4F4E-A4D5-03CD258B2FC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" activeCellId="2" sqref="A15:XFD15 A16:XFD16 A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1948,80 +1948,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="C12" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="C15" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="9" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the filename for previously written programs
</commit_message>
<xml_diff>
--- a/Questions/Questions.xlsx
+++ b/Questions/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\GitHub\Programming\Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845B0EF-2C52-434B-A2AE-059149A1CEF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14C596-7231-4ABC-BD37-DA57BAFA943D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1900,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A112" activeCellId="1" sqref="A111:XFD111 A112:XFD112"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2586,7 +2586,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2597,7 +2597,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2608,7 +2608,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2619,7 +2619,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2630,7 +2630,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2641,7 +2641,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2652,7 +2652,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2663,7 +2663,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2674,7 +2674,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2685,7 +2685,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>0</v>
+        <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2696,7 +2696,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2707,7 +2707,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2718,7 +2718,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2729,7 +2729,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2740,7 +2740,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2751,7 +2751,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2762,7 +2762,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>0</v>
+        <v>464</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2784,7 +2784,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>0</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2795,7 +2795,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2806,7 +2806,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -2817,7 +2817,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>0</v>
+        <v>460</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2828,7 +2828,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2839,7 +2839,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2850,7 +2850,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2861,7 +2861,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -2872,7 +2872,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>0</v>
+        <v>460</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -2883,7 +2883,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>0</v>
+        <v>460</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2894,7 +2894,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2905,7 +2905,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -2921,7 +2921,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2932,7 +2932,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2943,7 +2943,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2954,7 +2954,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2965,7 +2965,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2976,7 +2976,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>0</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2987,7 +2987,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -2998,7 +2998,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3009,7 +3009,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3020,7 +3020,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3031,7 +3031,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3042,7 +3042,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="108" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3053,7 +3053,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3064,7 +3064,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="110" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3075,7 +3075,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -3086,40 +3086,40 @@
         <v>109</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>0</v>
+        <v>461</v>
       </c>
     </row>
     <row r="112" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A112" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" s="21" t="s">
         <v>110</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A113" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
+      <c r="C113" s="9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A114" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>0</v>
+      <c r="C114" s="9" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Till 119 and created decorators.py
</commit_message>
<xml_diff>
--- a/Questions/Questions.xlsx
+++ b/Questions/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\GitHub\Programming\Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14C596-7231-4ABC-BD37-DA57BAFA943D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2A6B64-967A-4E58-8FAF-7CF3F712B5BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1900,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A119" activeCellId="2" sqref="A117:XFD117 A118:XFD118 A119:XFD119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3133,47 +3133,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A116" s="2" t="s">
+    <row r="116" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A116" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
+      <c r="C116" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A117" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A118" s="2" t="s">
+      <c r="C117" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A118" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A119" s="2" t="s">
+      <c r="C118" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A119" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="9" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>